<commit_message>
Change color indeces to start from 0
</commit_message>
<xml_diff>
--- a/colors.xlsx
+++ b/colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naren\Documents\UChicago\Clubs\UCES\LegoProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79999DD4-8638-4C7F-9907-1C5B6A4A7D53}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7531846A-5603-4039-99A4-01959E3FBEC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5004" yWindow="96" windowWidth="17280" windowHeight="8964" xr2:uid="{61DA2CAE-3A2C-4283-B98D-933F8C324BA6}"/>
+    <workbookView xWindow="3492" yWindow="4020" windowWidth="17280" windowHeight="8964" xr2:uid="{61DA2CAE-3A2C-4283-B98D-933F8C324BA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>